<commit_message>
geração de md - novas colunas para série temporal
</commit_message>
<xml_diff>
--- a/analises/2023/serie_temporal/dados/serie_por_modalidade_aon_2023.xlsx
+++ b/analises/2023/serie_temporal/dados/serie_por_modalidade_aon_2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ano</t>
   </si>
@@ -25,13 +25,34 @@
     <t>total_sucesso</t>
   </si>
   <si>
+    <t>particip</t>
+  </si>
+  <si>
+    <t>taxa_sucesso</t>
+  </si>
+  <si>
     <t>arrecadado_sucesso</t>
   </si>
   <si>
-    <t>taxa_sucesso</t>
-  </si>
-  <si>
     <t>media_sucesso</t>
+  </si>
+  <si>
+    <t>std_sucesso</t>
+  </si>
+  <si>
+    <t>min_sucesso</t>
+  </si>
+  <si>
+    <t>max_sucesso</t>
+  </si>
+  <si>
+    <t>apoio_medio</t>
+  </si>
+  <si>
+    <t>contribuicoes</t>
+  </si>
+  <si>
+    <t>media_contribuicoes</t>
   </si>
 </sst>
 </file>
@@ -39,8 +60,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="R$ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="164" formatCode="0.00%"/>
+    <numFmt numFmtId="165" formatCode="R$ #,##0.00"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -395,18 +416,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -425,8 +446,29 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -436,17 +478,38 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2">
         <v>61541.40151322056</v>
       </c>
-      <c r="E2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="G2" s="2">
         <v>61541.40151322056</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>61541.40151322056</v>
+      </c>
+      <c r="J2">
+        <v>61541.40151322056</v>
+      </c>
+      <c r="K2">
+        <v>107.7782863629082</v>
+      </c>
+      <c r="L2">
+        <v>571</v>
+      </c>
+      <c r="M2">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2012</v>
       </c>
@@ -456,17 +519,38 @@
       <c r="C3">
         <v>16</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1">
+        <v>72.72727272727273</v>
+      </c>
+      <c r="F3" s="2">
         <v>479445.0384204207</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.7272727272727273</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="G3" s="2">
         <v>29965.31490127629</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3">
+        <v>32844.83529194843</v>
+      </c>
+      <c r="I3">
+        <v>584.9223719501611</v>
+      </c>
+      <c r="J3">
+        <v>127701.0746790686</v>
+      </c>
+      <c r="K3">
+        <v>119.3540050835003</v>
+      </c>
+      <c r="L3">
+        <v>4017</v>
+      </c>
+      <c r="M3">
+        <v>251.0625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>2013</v>
       </c>
@@ -476,17 +560,38 @@
       <c r="C4">
         <v>43</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="1">
+        <v>81.13207547169812</v>
+      </c>
+      <c r="F4" s="2">
         <v>1428792.739081105</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.8113207547169812</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="G4" s="2">
         <v>33227.73811816523</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4">
+        <v>24965.31440121488</v>
+      </c>
+      <c r="I4">
+        <v>5106.24123472569</v>
+      </c>
+      <c r="J4">
+        <v>111934.9031053756</v>
+      </c>
+      <c r="K4">
+        <v>107.0336908443408</v>
+      </c>
+      <c r="L4">
+        <v>13349</v>
+      </c>
+      <c r="M4">
+        <v>310.4418604651163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>2014</v>
       </c>
@@ -496,17 +601,38 @@
       <c r="C5">
         <v>38</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1">
+        <v>61.29032258064516</v>
+      </c>
+      <c r="F5" s="2">
         <v>1162805.479251014</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.6129032258064516</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="G5" s="2">
         <v>30600.14419081615</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5">
+        <v>15792.34208006278</v>
+      </c>
+      <c r="I5">
+        <v>6709.995401213501</v>
+      </c>
+      <c r="J5">
+        <v>69031.34520734013</v>
+      </c>
+      <c r="K5">
+        <v>97.55897971734321</v>
+      </c>
+      <c r="L5">
+        <v>11919</v>
+      </c>
+      <c r="M5">
+        <v>313.6578947368421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>2015</v>
       </c>
@@ -516,17 +642,38 @@
       <c r="C6">
         <v>69</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6" s="1">
+        <v>51.8796992481203</v>
+      </c>
+      <c r="F6" s="2">
         <v>1819271.369997717</v>
       </c>
-      <c r="E6" s="2">
-        <v>0.518796992481203</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="G6" s="2">
         <v>26366.25173909736</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6">
+        <v>21171.78749083746</v>
+      </c>
+      <c r="I6">
+        <v>4045.018742516635</v>
+      </c>
+      <c r="J6">
+        <v>93151.10566503338</v>
+      </c>
+      <c r="K6">
+        <v>80.39912365201155</v>
+      </c>
+      <c r="L6">
+        <v>22628</v>
+      </c>
+      <c r="M6">
+        <v>327.9420289855072</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>2016</v>
       </c>
@@ -536,17 +683,38 @@
       <c r="C7">
         <v>72</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" s="1">
+        <v>57.59999999999999</v>
+      </c>
+      <c r="F7" s="2">
         <v>1624270.032475763</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.576</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="G7" s="2">
         <v>22559.30600660781</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7">
+        <v>16308.48437594153</v>
+      </c>
+      <c r="I7">
+        <v>4453.815556604946</v>
+      </c>
+      <c r="J7">
+        <v>81695.28923210928</v>
+      </c>
+      <c r="K7">
+        <v>76.47222375121292</v>
+      </c>
+      <c r="L7">
+        <v>21240</v>
+      </c>
+      <c r="M7">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>2017</v>
       </c>
@@ -556,17 +724,38 @@
       <c r="C8">
         <v>81</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1">
+        <v>58.27338129496403</v>
+      </c>
+      <c r="F8" s="2">
         <v>2087954.290163239</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.5827338129496403</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="G8" s="2">
         <v>25777.21345880542</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8">
+        <v>45696.71408523963</v>
+      </c>
+      <c r="I8">
+        <v>972.8163723722644</v>
+      </c>
+      <c r="J8">
+        <v>396557.4961875453</v>
+      </c>
+      <c r="K8">
+        <v>81.67557073084176</v>
+      </c>
+      <c r="L8">
+        <v>25564</v>
+      </c>
+      <c r="M8">
+        <v>315.604938271605</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -576,17 +765,38 @@
       <c r="C9">
         <v>99</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1">
+        <v>61.11111111111111</v>
+      </c>
+      <c r="F9" s="2">
         <v>2032376.432832572</v>
       </c>
-      <c r="E9" s="2">
-        <v>0.6111111111111112</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="G9" s="2">
         <v>20529.05487709669</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9">
+        <v>24451.8500186853</v>
+      </c>
+      <c r="I9">
+        <v>54.53892516702949</v>
+      </c>
+      <c r="J9">
+        <v>218217.2310776762</v>
+      </c>
+      <c r="K9">
+        <v>82.11953746949662</v>
+      </c>
+      <c r="L9">
+        <v>24749</v>
+      </c>
+      <c r="M9">
+        <v>249.989898989899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>2019</v>
       </c>
@@ -596,17 +806,38 @@
       <c r="C10">
         <v>101</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10" s="1">
+        <v>61.96319018404908</v>
+      </c>
+      <c r="F10" s="2">
         <v>2433333.565237989</v>
       </c>
-      <c r="E10" s="2">
-        <v>0.6196319018404908</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="G10" s="2">
         <v>24092.41153700979</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10">
+        <v>18933.09008805051</v>
+      </c>
+      <c r="I10">
+        <v>2765.732081374212</v>
+      </c>
+      <c r="J10">
+        <v>85065.08018876649</v>
+      </c>
+      <c r="K10">
+        <v>79.16369201763254</v>
+      </c>
+      <c r="L10">
+        <v>30738</v>
+      </c>
+      <c r="M10">
+        <v>304.3366336633663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -616,17 +847,38 @@
       <c r="C11">
         <v>66</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11" s="1">
+        <v>64.07766990291263</v>
+      </c>
+      <c r="F11" s="2">
         <v>2133850.109966084</v>
       </c>
-      <c r="E11" s="2">
-        <v>0.6407766990291263</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="G11" s="2">
         <v>32331.0622722134</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="H11">
+        <v>37494.77850275363</v>
+      </c>
+      <c r="I11">
+        <v>787.1021772339901</v>
+      </c>
+      <c r="J11">
+        <v>163173.270269744</v>
+      </c>
+      <c r="K11">
+        <v>98.35676930011913</v>
+      </c>
+      <c r="L11">
+        <v>21695</v>
+      </c>
+      <c r="M11">
+        <v>328.7121212121212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -636,17 +888,38 @@
       <c r="C12">
         <v>67</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12" s="1">
+        <v>64.42307692307693</v>
+      </c>
+      <c r="F12" s="2">
         <v>3217184.860207676</v>
       </c>
-      <c r="E12" s="2">
-        <v>0.6442307692307693</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="G12" s="2">
         <v>48017.68448071158</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="H12">
+        <v>94193.53461142223</v>
+      </c>
+      <c r="I12">
+        <v>94.898114598278</v>
+      </c>
+      <c r="J12">
+        <v>679297.6600721752</v>
+      </c>
+      <c r="K12">
+        <v>102.7362241803505</v>
+      </c>
+      <c r="L12">
+        <v>31315</v>
+      </c>
+      <c r="M12">
+        <v>467.3880597014925</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>2022</v>
       </c>
@@ -656,17 +929,38 @@
       <c r="C13">
         <v>81</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13" s="1">
+        <v>60.90225563909775</v>
+      </c>
+      <c r="F13" s="2">
         <v>2345603.516727894</v>
       </c>
-      <c r="E13" s="2">
-        <v>0.6090225563909775</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="G13" s="2">
         <v>28958.06810775177</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13">
+        <v>48382.24972145099</v>
+      </c>
+      <c r="I13">
+        <v>41.81688448509265</v>
+      </c>
+      <c r="J13">
+        <v>264585.9073482947</v>
+      </c>
+      <c r="K13">
+        <v>97.31583274811823</v>
+      </c>
+      <c r="L13">
+        <v>24103</v>
+      </c>
+      <c r="M13">
+        <v>297.5679012345679</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>2023</v>
       </c>
@@ -676,14 +970,35 @@
       <c r="C14">
         <v>96</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14" s="1">
+        <v>71.64179104477611</v>
+      </c>
+      <c r="F14" s="2">
         <v>3236850.991448335</v>
       </c>
-      <c r="E14" s="2">
-        <v>0.7164179104477612</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="G14" s="2">
         <v>33717.19782758682</v>
+      </c>
+      <c r="H14">
+        <v>65399.89171729227</v>
+      </c>
+      <c r="I14">
+        <v>721.7894130003107</v>
+      </c>
+      <c r="J14">
+        <v>537544.5528256212</v>
+      </c>
+      <c r="K14">
+        <v>102.2217271892732</v>
+      </c>
+      <c r="L14">
+        <v>31665</v>
+      </c>
+      <c r="M14">
+        <v>329.84375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>